<commit_message>
Adding XLS Support to Excel Utils
</commit_message>
<xml_diff>
--- a/src/test/resources/Excel Files/testGoogle.xlsx
+++ b/src/test/resources/Excel Files/testGoogle.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="testGoogle" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>TestCase ID</t>
   </si>
@@ -47,6 +47,18 @@
   </si>
   <si>
     <t>Antony_Password</t>
+  </si>
+  <si>
+    <t>TC_003</t>
+  </si>
+  <si>
+    <t>TRUE</t>
+  </si>
+  <si>
+    <t>10000100</t>
+  </si>
+  <si>
+    <t>10002</t>
   </si>
 </sst>
 </file>
@@ -111,10 +123,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -395,16 +408,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.28515625" customWidth="1"/>
     <col min="4" max="16384" width="9.140625" hidden="1"/>
   </cols>
@@ -442,6 +455,28 @@
         <v>8</v>
       </c>
     </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -452,7 +487,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>

<commit_message>
Modified the Code to work with latest dependencies
</commit_message>
<xml_diff>
--- a/src/test/resources/Excel Files/testGoogle.xlsx
+++ b/src/test/resources/Excel Files/testGoogle.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29530"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54CDACAC-67A6-46BC-AEE2-075F9B27E779}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="testGoogle" sheetId="1" r:id="rId1"/>
@@ -64,7 +65,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -127,7 +128,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -407,11 +408,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -484,7 +485,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>